<commit_message>
"for add git remote"
</commit_message>
<xml_diff>
--- a/git.xlsx
+++ b/git.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>WORK</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -107,10 +107,6 @@
   </si>
   <si>
     <t>克隆项目：</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>git clone git@github.com:seidogao/learngit2018</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -134,6 +130,20 @@
   </si>
   <si>
     <t>Warning: Permanently added 'github.com' (RSA) to the list of known hosts.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">origin  git@github.com:seidogao/learngit2018 (fetch)
+origin  git@github.com:seidogao/learngit2018 (push)
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$ git clone git@github.com:seidogao/learngit2018</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$ git remote -v</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -369,7 +379,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -423,6 +433,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1603,7 +1616,7 @@
   <dimension ref="B1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -1786,16 +1799,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:J24"/>
+  <dimension ref="A2:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
   <cols>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="37" customWidth="1"/>
+    <col min="2" max="2" width="49.28515625" customWidth="1"/>
+    <col min="3" max="3" width="58" customWidth="1"/>
     <col min="10" max="10" width="64.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1887,27 +1900,40 @@
     </row>
     <row r="21" spans="1:3">
       <c r="B21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="B22" s="16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="36">
+      <c r="C23" s="18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="72">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="15" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="72">
-      <c r="A23" t="s">
+      <c r="C24" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="B25" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="B24" t="s">
+      <c r="C25" t="s">
         <v>27</v>
       </c>
-      <c r="C24" t="s">
-        <v>28</v>
-      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="B29" s="15"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>